<commit_message>
Correções no cruzamento de dados e estilização de Exel
</commit_message>
<xml_diff>
--- a/PrototipoAnapolis/RelatórioFinal.xlsx
+++ b/PrototipoAnapolis/RelatórioFinal.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>Observação</t>
   </si>
@@ -97,15 +97,12 @@
     <t>Frente:14,00m                     Confrontando com Rua Tarsila do Amaral     Fundo:14,00m                     Confrontando com Lote 23(Vinte e trï¿½s)      Lado Direito:30,00m            Confrontando com Lote 18(Dezoito)        Lado Esquerdo: 30,00m      Confrontando com Lote 16(Dezesseis)</t>
   </si>
   <si>
-    <t xml:space="preserve"> Totais</t>
+    <t>Totais R$:</t>
   </si>
   <si>
     <t>105.322.0262.000</t>
   </si>
   <si>
-    <t>R$:</t>
-  </si>
-  <si>
     <t>13</t>
   </si>
   <si>
@@ -133,7 +130,13 @@
     <t>Condominio Residencial Belas Artes</t>
   </si>
   <si>
+    <t>Q13 Lt017</t>
+  </si>
+  <si>
     <t>Vendido</t>
+  </si>
+  <si>
+    <t>81-013-0017E</t>
   </si>
   <si>
     <t>Solimar Inacio de Bastos</t>
@@ -146,7 +149,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -158,14 +161,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -186,7 +181,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF666666"/>
+        <fgColor rgb="FFC6E2FF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -226,7 +221,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -535,10 +530,14 @@
     <col min="9" max="9" width="14.7109375" customWidth="1"/>
     <col min="10" max="10" width="10.7109375" customWidth="1"/>
     <col min="13" max="13" width="10.7109375" customWidth="1"/>
-    <col min="16" max="16" width="32.7109375" customWidth="1"/>
+    <col min="16" max="16" width="28.7109375" customWidth="1"/>
     <col min="17" max="17" width="12.7109375" customWidth="1"/>
-    <col min="18" max="18" width="32.7109375" customWidth="1"/>
+    <col min="18" max="18" width="28.7109375" customWidth="1"/>
     <col min="19" max="19" width="20.7109375" customWidth="1"/>
+    <col min="20" max="20" width="12.7109375" customWidth="1"/>
+    <col min="21" max="22" width="18.7109375" customWidth="1"/>
+    <col min="24" max="24" width="28.7109375" customWidth="1"/>
+    <col min="25" max="26" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26">
@@ -629,25 +628,25 @@
         <v>28</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>36</v>
       </c>
       <c r="J2" s="2">
         <v>3008.01</v>
@@ -668,36 +667,39 @@
         <v>14</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="Q2" s="2">
         <v>56</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="S2" s="2">
         <v>81</v>
       </c>
+      <c r="T2" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="U2" s="2" t="s">
         <v>39</v>
       </c>
+      <c r="V2" s="2" t="s">
+        <v>40</v>
+      </c>
       <c r="W2" s="2">
         <v>13548</v>
       </c>
       <c r="X2" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="Y2" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:26" s="3" customFormat="1">
       <c r="A3" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>29</v>
       </c>
       <c r="J3" s="3">
         <v>3008.01</v>

</xml_diff>

<commit_message>
Adição de novos campos ao exel e atualização de dados.
</commit_message>
<xml_diff>
--- a/PrototipoAnapolis/RelatórioFinal.xlsx
+++ b/PrototipoAnapolis/RelatórioFinal.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t>Observação</t>
   </si>
@@ -94,6 +94,12 @@
     <t>CNPJ</t>
   </si>
   <si>
+    <t>Área Priv.</t>
+  </si>
+  <si>
+    <t>Área Com.</t>
+  </si>
+  <si>
     <t>Frente:14,00m                     Confrontando com Rua Tarsila do Amaral     Fundo:14,00m                     Confrontando com Lote 23(Vinte e trï¿½s)      Lado Direito:30,00m            Confrontando com Lote 18(Dezoito)        Lado Esquerdo: 30,00m      Confrontando com Lote 16(Dezesseis)</t>
   </si>
   <si>
@@ -143,6 +149,12 @@
   </si>
   <si>
     <t>Anapolis</t>
+  </si>
+  <si>
+    <t>420</t>
+  </si>
+  <si>
+    <t>364,29</t>
   </si>
 </sst>
 </file>
@@ -518,7 +530,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Z3"/>
+  <dimension ref="A1:AB3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -540,7 +552,7 @@
     <col min="25" max="26" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26">
+    <row r="1" spans="1:28">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -619,34 +631,40 @@
       <c r="Z1" s="1" t="s">
         <v>25</v>
       </c>
+      <c r="AA1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="2" spans="1:26" s="2" customFormat="1">
+    <row r="2" spans="1:28" s="2" customFormat="1">
       <c r="A2" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="J2" s="2">
         <v>3008.01</v>
@@ -667,39 +685,45 @@
         <v>14</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="Q2" s="2">
         <v>56</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="S2" s="2">
         <v>81</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="U2" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="V2" s="2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="W2" s="2">
         <v>13548</v>
       </c>
       <c r="X2" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="Y2" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
+      </c>
+      <c r="AA2" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB2" s="2" t="s">
+        <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:26" s="3" customFormat="1">
+    <row r="3" spans="1:28" s="3" customFormat="1">
       <c r="A3" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="J3" s="3">
         <v>3008.01</v>

</xml_diff>